<commit_message>
STX C1/C2 -> STX_C1/C2, STX C1/C2 -> STX_C3/C4
</commit_message>
<xml_diff>
--- a/config/lista_toxiner.xlsx
+++ b/config/lista_toxiner.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\SLV-Biotoxin-Validator-App\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anderstorstensson/Dropbox/R/SLV-Biotoxin-Validator-App/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F22D506-7905-4FA1-A77E-A6A13959047F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3E57F3-39CD-9D45-9C2B-B133671167F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{5EE10D2C-8E1B-4393-ADF2-C1365B6C7898}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="18640" xr2:uid="{5EE10D2C-8E1B-4393-ADF2-C1365B6C7898}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$O$48</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -612,12 +612,6 @@
     <t>45_OH_YTX</t>
   </si>
   <si>
-    <t>STX C1_C2</t>
-  </si>
-  <si>
-    <t>STX C3_C4</t>
-  </si>
-  <si>
     <t>dcGTX2_dcGTX3</t>
   </si>
   <si>
@@ -1057,6 +1051,12 @@
   </si>
   <si>
     <t>Merge_MH</t>
+  </si>
+  <si>
+    <t>STX_C3_C4</t>
+  </si>
+  <si>
+    <t>STX_C1_C2</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1187,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1485,34 +1485,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{604718B0-4585-451D-AFD3-6923AD565DA1}">
   <dimension ref="A1:S72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" topLeftCell="L3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" customWidth="1"/>
-    <col min="6" max="6" width="46.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.1796875" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" customWidth="1"/>
-    <col min="10" max="10" width="3.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.453125" customWidth="1"/>
-    <col min="13" max="13" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="43.453125" customWidth="1"/>
-    <col min="15" max="15" width="25.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="46.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.5" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="43.5" customWidth="1"/>
+    <col min="15" max="15" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>182</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>83</v>
@@ -1562,16 +1562,16 @@
         <v>190</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>45OH_carboxyYTX (mg YTX eq/kg)</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>45_OH_homoYTX (mg YTX eq/kg)</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>45_OH_YTX (mg YTX eq/kg)</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>DA (mg/kg)</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>AZA1 (ug AZA eq/kg)</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>AZA2 (ug AZA eq/kg)</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>AZA3 (ug AZA eq/kg)</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -2006,10 +2006,10 @@
         <v>45691</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>185</v>
@@ -2019,7 +2019,7 @@
         <v>AZA_tot (ug AZA eq/kg)</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>162</v>
       </c>
@@ -2052,20 +2052,20 @@
       <c r="N10" s="4"/>
       <c r="O10" s="5"/>
       <c r="P10" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q10" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="Q10" s="7" t="s">
-        <v>291</v>
-      </c>
       <c r="R10" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S10" t="str">
         <f t="shared" si="0"/>
         <v>C1_2 (true or false)</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
@@ -2108,20 +2108,20 @@
         <v>45691</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>194</v>
+        <v>342</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>186</v>
       </c>
       <c r="S11" t="str">
         <f t="shared" si="0"/>
-        <v>STX C1_C2 (ug STXdiHCL eq/kg)</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+        <v>STX_C1_C2 (ug STXdiHCL eq/kg)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>174</v>
       </c>
@@ -2143,20 +2143,20 @@
       <c r="M12" s="4"/>
       <c r="O12" s="5"/>
       <c r="P12" s="11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="Q12" s="11" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="S12" t="str">
         <f t="shared" si="0"/>
         <v>C3_4 (Unit)</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
@@ -2197,20 +2197,20 @@
         <v>45691</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>195</v>
+        <v>341</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>186</v>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="0"/>
-        <v>STX C3_C4 (ug STXdiHCL eq/kg)</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+        <v>STX_C3_C4 (ug STXdiHCL eq/kg)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>CarboxyYTX (mg YTX eq/kg)</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>169</v>
       </c>
@@ -2283,20 +2283,20 @@
         <v>54</v>
       </c>
       <c r="P15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="Q15" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="0"/>
         <v>dcGTX2_3_screen_pos (true or false)</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
@@ -2339,10 +2339,10 @@
         <v>45691</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="R16" s="4" t="s">
         <v>186</v>
@@ -2352,7 +2352,7 @@
         <v>dcGTX2_dcGTX3 (ug STXdiHCL eq/kg)</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>171</v>
       </c>
@@ -2369,20 +2369,20 @@
         <v>54</v>
       </c>
       <c r="P17" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="Q17" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="0"/>
         <v>dcNEO_screen_pos (true or false)</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>31</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>dcNeoSTX (ug STXdiHCL eq/kg)</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
@@ -2461,20 +2461,20 @@
         <v>54</v>
       </c>
       <c r="P19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="Q19" s="12" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S19" t="str">
         <f t="shared" si="0"/>
         <v>dcSTX_screen_pos (true or false)</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>33</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>dcSTX (ug STXdiHCL eq/kg)</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>173</v>
       </c>
@@ -2553,20 +2553,20 @@
       <c r="N21" s="4"/>
       <c r="O21" s="5"/>
       <c r="P21" s="11" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Q21" s="11" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="S21" t="str">
         <f t="shared" si="0"/>
         <v>DA_LP205 (Unit)</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>12</v>
       </c>
@@ -2603,20 +2603,20 @@
         <v>45691</v>
       </c>
       <c r="P22" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Q22" s="7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S22" t="str">
         <f t="shared" si="0"/>
         <v>DA_screen_pos (true or false)</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>13</v>
       </c>
@@ -2654,10 +2654,10 @@
         <v>45691</v>
       </c>
       <c r="P23" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="Q23" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="R23" s="4" t="s">
         <v>187</v>
@@ -2667,7 +2667,7 @@
         <v>DST_tot (ug OA eq/kg)</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>14</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>DTX1 (ug OA eq/kg)</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>15</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>DTX3 (ug OA eq/kg)</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>DTX2 (ug OA eq/kg)</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>17</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>111</v>
       </c>
       <c r="Q27" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R27" s="4" t="s">
         <v>187</v>
@@ -2884,7 +2884,7 @@
         <v>DTX2_acyl (ug OA eq/kg)</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>27</v>
       </c>
@@ -2917,10 +2917,10 @@
       <c r="N28" s="4"/>
       <c r="O28" s="5"/>
       <c r="P28" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q28" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="R28" s="4" t="s">
         <v>161</v>
@@ -2930,7 +2930,7 @@
         <v>E_coli (cells/100 g)</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>35</v>
       </c>
@@ -2957,20 +2957,20 @@
       <c r="N29" s="4"/>
       <c r="O29" s="5"/>
       <c r="P29" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="Q29" s="7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S29" t="str">
         <f t="shared" si="0"/>
         <v>GTX1_4_screen_pos (true or false)</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>34</v>
       </c>
@@ -3013,10 +3013,10 @@
         <v>45691</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Q30" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>186</v>
@@ -3026,7 +3026,7 @@
         <v>GTX1_GTX4 (ug STXdiHCL eq/kg)</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>36</v>
       </c>
@@ -3049,20 +3049,20 @@
         <v>54</v>
       </c>
       <c r="P31" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="Q31" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="R31" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S31" t="str">
         <f t="shared" si="0"/>
         <v>GTX2_3_screen_pos (true or false)</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>37</v>
       </c>
@@ -3105,10 +3105,10 @@
         <v>45691</v>
       </c>
       <c r="P32" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Q32" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="R32" s="4" t="s">
         <v>186</v>
@@ -3118,7 +3118,7 @@
         <v>GTX2_GTX3 (ug STXdiHCL eq/kg)</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>38</v>
       </c>
@@ -3141,20 +3141,20 @@
         <v>54</v>
       </c>
       <c r="P33" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Q33" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R33" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S33" t="str">
         <f t="shared" si="0"/>
         <v>GTX5_screen_pos (true or false)</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>39</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>GTX5 (ug STXdiHCL eq/kg)</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>41</v>
       </c>
@@ -3233,20 +3233,20 @@
         <v>54</v>
       </c>
       <c r="P35" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="Q35" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S35" t="str">
         <f t="shared" si="0"/>
         <v>GTX6_screen_pos (true or false)</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>40</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>GTX6 (ug STXdiHCL eq/kg)</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>18</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>HomoYTX (mg YTX eq/kg)</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>175</v>
       </c>
@@ -3379,20 +3379,20 @@
       <c r="N38" s="4"/>
       <c r="O38" s="5"/>
       <c r="P38" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="Q38" s="11" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="R38" s="11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="S38" t="str">
         <f t="shared" si="0"/>
         <v>Shortname (Unit)</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>42</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>NeoSTX (ug STXdiHCL eq/kg)</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>19</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>110</v>
       </c>
       <c r="Q40" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="R40" s="4" t="s">
         <v>187</v>
@@ -3498,7 +3498,7 @@
         <v>OA_acyl (ug OA eq/kg)</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>20</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>Okadaic acid (ug OA eq/kg)</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>176</v>
       </c>
@@ -3579,20 +3579,20 @@
       <c r="N42" s="4"/>
       <c r="O42" s="5"/>
       <c r="P42" s="11" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Q42" s="11" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="R42" s="11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="S42" t="str">
         <f t="shared" si="0"/>
         <v>PSP_tot (Unit)</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>43</v>
       </c>
@@ -3629,10 +3629,10 @@
       <c r="N43" s="4"/>
       <c r="O43" s="5"/>
       <c r="P43" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="Q43" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="R43" s="4" t="s">
         <v>186</v>
@@ -3642,7 +3642,7 @@
         <v>PST_tot (ug STXdiHCL eq/kg)</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>21</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>PTX1 (ug PTX eq/kg)</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>22</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>PTX2 (ug PTX eq/kg)</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>23</v>
       </c>
@@ -3791,10 +3791,10 @@
         <v>45691</v>
       </c>
       <c r="P46" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="Q46" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="R46" s="4" t="s">
         <v>188</v>
@@ -3804,7 +3804,7 @@
         <v>PTX_tot (ug PTX eq/kg)</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>24</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>SPX1 (ug/kg)</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>44</v>
       </c>
@@ -3869,20 +3869,20 @@
         <v>54</v>
       </c>
       <c r="P48" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="Q48" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="R48" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S48" t="str">
         <f t="shared" si="0"/>
         <v>STX_screen_pos (true or false)</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>45</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>STX (ug STXdiHCL eq/kg)</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>25</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>YTX (mg YTX eq/kg)</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>26</v>
       </c>
@@ -4037,10 +4037,10 @@
         <v>53</v>
       </c>
       <c r="P51" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="Q51" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="R51" s="4" t="s">
         <v>67</v>
@@ -4050,24 +4050,24 @@
         <v>YTX_tot (mg YTX eq/kg)</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>184</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="M52" t="s">
         <v>50</v>
       </c>
       <c r="P52" s="10" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="Q52" s="10" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="R52" s="16" t="s">
         <v>50</v>
@@ -4077,24 +4077,24 @@
         <v>Ana_a (mg/kg)</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>184</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="M53" t="s">
         <v>50</v>
       </c>
       <c r="P53" s="10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="Q53" s="10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="R53" s="16" t="s">
         <v>50</v>
@@ -4104,45 +4104,45 @@
         <v>h_Ana (mg/kg)</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>184</v>
       </c>
       <c r="D54" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E54" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="F54" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="F54" s="4" t="s">
-        <v>256</v>
-      </c>
       <c r="G54" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="M54" t="s">
         <v>50</v>
       </c>
       <c r="N54" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="O54" s="5">
         <v>45698</v>
       </c>
       <c r="P54" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="Q54" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="R54" s="16" t="s">
         <v>50</v>
@@ -4152,45 +4152,45 @@
         <v>CYN (mg/kg)</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C55" t="s">
         <v>184</v>
       </c>
       <c r="D55" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E55" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F55" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="M55" t="s">
         <v>50</v>
       </c>
       <c r="N55" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="O55" s="5">
         <v>45700</v>
       </c>
       <c r="P55" s="10" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="Q55" s="10" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="R55" s="16" t="s">
         <v>50</v>
@@ -4200,45 +4200,45 @@
         <v>MC_HTyR (mg/kg)</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C56" t="s">
         <v>184</v>
       </c>
       <c r="D56" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E56" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F56" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G56" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="K56" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="L56" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="M56" t="s">
         <v>50</v>
       </c>
       <c r="N56" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="O56" s="5">
         <v>45700</v>
       </c>
       <c r="P56" s="14" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Q56" s="10" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="R56" s="16" t="s">
         <v>50</v>
@@ -4248,45 +4248,45 @@
         <v>MC_LR_D_Asp3 (mg/kg)</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C57" t="s">
         <v>184</v>
       </c>
       <c r="D57" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E57" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F57" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G57" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="K57" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="L57" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="M57" t="s">
         <v>50</v>
       </c>
       <c r="N57" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="O57" s="5">
         <v>45700</v>
       </c>
       <c r="P57" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="Q57" s="10" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="R57" s="16" t="s">
         <v>50</v>
@@ -4296,45 +4296,45 @@
         <v>MC_RR_D_Asp3 (mg/kg)</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C58" t="s">
         <v>184</v>
       </c>
       <c r="D58" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E58" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F58" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G58" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="K58" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L58" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="M58" s="3" t="s">
         <v>50</v>
       </c>
       <c r="N58" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="O58" s="5">
         <v>45700</v>
       </c>
       <c r="P58" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="Q58" s="10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="R58" s="16" t="s">
         <v>50</v>
@@ -4344,48 +4344,48 @@
         <v>NOD_R (mg/kg)</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C59" t="s">
         <v>184</v>
       </c>
       <c r="D59" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E59" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F59" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="M59" s="3" t="s">
         <v>50</v>
       </c>
       <c r="N59" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="O59" s="5">
         <v>45698</v>
       </c>
       <c r="P59" s="15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="Q59" s="15" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="R59" s="3" t="s">
         <v>50</v>
@@ -4395,45 +4395,45 @@
         <v>MC_RR (mg/kg)</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C60" t="s">
         <v>184</v>
       </c>
       <c r="D60" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E60" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G60" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K60" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L60" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="M60" t="s">
         <v>50</v>
       </c>
       <c r="N60" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="O60" s="5">
         <v>45698</v>
       </c>
       <c r="P60" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="Q60" s="10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="R60" t="s">
         <v>50</v>
@@ -4443,45 +4443,45 @@
         <v>MC_LR (mg/kg)</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C61" t="s">
         <v>184</v>
       </c>
       <c r="D61" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E61" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F61" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G61" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K61" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L61" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="M61" t="s">
         <v>50</v>
       </c>
       <c r="N61" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="O61" s="5">
         <v>45698</v>
       </c>
       <c r="P61" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="Q61" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="R61" t="s">
         <v>50</v>
@@ -4491,45 +4491,45 @@
         <v>MC_YR (mg/kg)</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C62" t="s">
         <v>184</v>
       </c>
       <c r="D62" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E62" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F62" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G62" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K62" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L62" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="M62" t="s">
         <v>50</v>
       </c>
       <c r="N62" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="O62" s="5">
         <v>45698</v>
       </c>
       <c r="P62" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="Q62" s="10" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="R62" t="s">
         <v>50</v>
@@ -4539,45 +4539,45 @@
         <v>MC_LA (mg/kg)</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C63" t="s">
         <v>184</v>
       </c>
       <c r="D63" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E63" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F63" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G63" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K63" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="L63" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="M63" t="s">
         <v>50</v>
       </c>
       <c r="N63" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="O63" s="5">
         <v>45698</v>
       </c>
       <c r="P63" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q63" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="R63" t="s">
         <v>50</v>
@@ -4587,45 +4587,45 @@
         <v>MC_LF (mg/kg)</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C64" t="s">
         <v>184</v>
       </c>
       <c r="D64" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E64" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F64" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G64" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="K64" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="L64" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M64" t="s">
         <v>50</v>
       </c>
       <c r="N64" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="O64" s="5">
         <v>45698</v>
       </c>
       <c r="P64" s="10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="Q64" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="R64" t="s">
         <v>50</v>
@@ -4635,45 +4635,45 @@
         <v>MC_LW (mg/kg)</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C65" t="s">
         <v>184</v>
       </c>
       <c r="D65" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E65" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F65" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G65" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="K65" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="L65" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M65" t="s">
         <v>50</v>
       </c>
       <c r="N65" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="O65" s="5">
         <v>45698</v>
       </c>
       <c r="P65" s="10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="Q65" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="R65" t="s">
         <v>50</v>
@@ -4683,45 +4683,45 @@
         <v>MC_LY (mg/kg)</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C66" t="s">
         <v>184</v>
       </c>
       <c r="D66" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E66" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F66" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G66" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="K66" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="L66" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="M66" t="s">
         <v>50</v>
       </c>
       <c r="N66" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="O66" s="5">
         <v>45698</v>
       </c>
       <c r="P66" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="Q66" s="10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="R66" t="s">
         <v>50</v>
@@ -4731,45 +4731,45 @@
         <v>MC_WR (mg/kg)</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C67" t="s">
         <v>184</v>
       </c>
       <c r="D67" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E67" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F67" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G67" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K67" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="L67" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="M67" t="s">
         <v>50</v>
       </c>
       <c r="N67" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="O67" s="5">
         <v>45698</v>
       </c>
       <c r="P67" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="Q67" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="R67" t="s">
         <v>50</v>
@@ -4779,30 +4779,30 @@
         <v>MC_HilR (mg/kg)</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C68" t="s">
         <v>184</v>
       </c>
       <c r="D68" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E68" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F68" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M68" t="s">
         <v>50</v>
       </c>
       <c r="P68" s="13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="Q68" s="13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="R68" t="s">
         <v>50</v>
@@ -4812,45 +4812,45 @@
         <v>MC_RR_D_Asp3_E_Dhb7 (mg/kg)</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C69" t="s">
         <v>184</v>
       </c>
       <c r="D69" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E69" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F69" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G69" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="K69" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="L69" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="M69" t="s">
         <v>50</v>
       </c>
       <c r="N69" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="O69" s="5">
         <v>45700</v>
       </c>
       <c r="P69" s="14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="Q69" s="14" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="R69" t="s">
         <v>50</v>
@@ -4860,45 +4860,45 @@
         <v>MC_LR_Dha7 (mg/kg)</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C70" t="s">
         <v>184</v>
       </c>
       <c r="D70" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E70" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F70" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G70" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="K70" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="L70" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M70" t="s">
         <v>50</v>
       </c>
       <c r="N70" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="O70" s="5">
         <v>45700</v>
       </c>
       <c r="P70" s="10" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="Q70" s="10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="R70" t="s">
         <v>50</v>
@@ -4908,30 +4908,30 @@
         <v>MC_RR_Dha7 (mg/kg)</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>248</v>
+      </c>
+      <c r="C71" t="s">
+        <v>184</v>
+      </c>
+      <c r="D71" t="s">
         <v>250</v>
       </c>
-      <c r="C71" t="s">
-        <v>184</v>
-      </c>
-      <c r="D71" t="s">
-        <v>252</v>
-      </c>
       <c r="E71" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F71" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M71" t="s">
         <v>50</v>
       </c>
       <c r="P71" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="Q71" s="10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="R71" t="s">
         <v>50</v>
@@ -4941,30 +4941,30 @@
         <v>MC_HphR_DAsp3_E_Dhb7 (mg/kg)</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C72" t="s">
         <v>184</v>
       </c>
       <c r="D72" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E72" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F72" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M72" t="s">
         <v>50</v>
       </c>
       <c r="P72" s="10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="Q72" s="10" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="R72" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
check PST and DA
</commit_message>
<xml_diff>
--- a/config/lista_toxiner.xlsx
+++ b/config/lista_toxiner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\SLV-Biotoxin-Validator-App\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64426ED3-1226-4CCB-8D12-F0333908F256}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6703E71A-1F0D-4464-823E-0F483F5B07B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17595" yWindow="495" windowWidth="33600" windowHeight="28275" xr2:uid="{5EE10D2C-8E1B-4393-ADF2-C1365B6C7898}"/>
   </bookViews>
@@ -1029,9 +1029,6 @@
     <t>[Dha7]MC-RR</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Merge_MH</t>
   </si>
   <si>
@@ -1122,13 +1119,16 @@
     <t>Decarbamoylsaxitoxin screening positive</t>
   </si>
   <si>
-    <t>Domoic acid screening</t>
-  </si>
-  <si>
     <t>DA_screening</t>
   </si>
   <si>
     <t>PST_tot_screen_pos</t>
+  </si>
+  <si>
+    <t>PST total screening positive</t>
+  </si>
+  <si>
+    <t>Domoic acid screening value</t>
   </si>
 </sst>
 </file>
@@ -1578,11 +1578,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{604718B0-4585-451D-AFD3-6923AD565DA1}">
   <dimension ref="A1:Y72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,13 +1616,13 @@
         <v>88</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>350</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>351</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>352</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>178</v>
@@ -1637,10 +1637,10 @@
         <v>83</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>349</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>91</v>
@@ -1679,13 +1679,13 @@
         <v>228</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
@@ -1753,13 +1753,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="D3" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>179</v>
@@ -1815,7 +1815,7 @@
         <v>185</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Y3" t="str">
         <f t="shared" si="0"/>
@@ -1827,13 +1827,13 @@
         <v>8</v>
       </c>
       <c r="B4" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>179</v>
@@ -1889,7 +1889,7 @@
         <v>185</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Y4" t="str">
         <f t="shared" si="0"/>
@@ -1901,13 +1901,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>179</v>
@@ -1963,7 +1963,7 @@
         <v>185</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Y5" t="str">
         <f t="shared" si="0"/>
@@ -1975,13 +1975,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D6" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>179</v>
@@ -2033,87 +2033,87 @@
         <v>185</v>
       </c>
       <c r="X6" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Y6" t="str">
         <f t="shared" si="0"/>
         <v>AZA_tot (ug AZA eq/kg)</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>353</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="D7" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>355</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="16">
         <v>3</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="16">
         <v>20</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="16">
         <v>1</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="Q7" s="4" t="s">
+      <c r="Q7" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S7" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="T7" s="5">
+      <c r="T7" s="19">
         <v>45688</v>
       </c>
-      <c r="U7" s="4" t="s">
+      <c r="U7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="V7" s="4" t="s">
+      <c r="V7" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="W7" s="4" t="s">
+      <c r="W7" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="X7" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="Y7" t="str">
+      <c r="X7" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="Y7" s="18" t="str">
         <f t="shared" si="0"/>
         <v>DA (mg/kg)</v>
       </c>
@@ -2123,13 +2123,13 @@
         <v>173</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>353</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="D8" s="17" t="s">
         <v>354</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>355</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>177</v>
@@ -2177,16 +2177,16 @@
         <v>12</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>353</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>355</v>
-      </c>
       <c r="E9" s="16" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>184</v>
@@ -2224,16 +2224,16 @@
         <v>45691</v>
       </c>
       <c r="U9" s="16" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="V9" s="16" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="W9" s="16" t="s">
         <v>50</v>
       </c>
       <c r="X9" s="16" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y9" s="18" t="str">
         <f t="shared" si="0"/>
@@ -2245,13 +2245,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="D10" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>179</v>
@@ -2302,7 +2302,7 @@
         <v>187</v>
       </c>
       <c r="X10" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Y10" t="str">
         <f t="shared" si="0"/>
@@ -2314,13 +2314,13 @@
         <v>14</v>
       </c>
       <c r="B11" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="D11" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>179</v>
@@ -2376,7 +2376,7 @@
         <v>187</v>
       </c>
       <c r="X11" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Y11" t="str">
         <f t="shared" si="0"/>
@@ -2388,13 +2388,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="D12" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>179</v>
@@ -2450,7 +2450,7 @@
         <v>187</v>
       </c>
       <c r="X12" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Y12" t="str">
         <f t="shared" si="0"/>
@@ -2462,13 +2462,13 @@
         <v>16</v>
       </c>
       <c r="B13" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="D13" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>179</v>
@@ -2524,7 +2524,7 @@
         <v>187</v>
       </c>
       <c r="X13" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="0"/>
@@ -2536,13 +2536,13 @@
         <v>17</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="D14" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>179</v>
@@ -2591,7 +2591,7 @@
         <v>187</v>
       </c>
       <c r="X14" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Y14" t="str">
         <f t="shared" si="0"/>
@@ -2603,13 +2603,13 @@
         <v>19</v>
       </c>
       <c r="B15" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>179</v>
@@ -2659,7 +2659,7 @@
         <v>187</v>
       </c>
       <c r="X15" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Y15" t="str">
         <f t="shared" si="0"/>
@@ -2671,13 +2671,13 @@
         <v>20</v>
       </c>
       <c r="B16" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="D16" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>179</v>
@@ -2735,7 +2735,7 @@
         <v>187</v>
       </c>
       <c r="X16" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Y16" t="str">
         <f t="shared" si="0"/>
@@ -2747,13 +2747,13 @@
         <v>21</v>
       </c>
       <c r="B17" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="D17" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>179</v>
@@ -2809,7 +2809,7 @@
         <v>188</v>
       </c>
       <c r="X17" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="Y17" t="str">
         <f t="shared" si="0"/>
@@ -2821,13 +2821,13 @@
         <v>22</v>
       </c>
       <c r="B18" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="D18" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>179</v>
@@ -2883,7 +2883,7 @@
         <v>188</v>
       </c>
       <c r="X18" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="Y18" t="str">
         <f t="shared" si="0"/>
@@ -2895,13 +2895,13 @@
         <v>23</v>
       </c>
       <c r="B19" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="D19" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>179</v>
@@ -2951,7 +2951,7 @@
         <v>188</v>
       </c>
       <c r="X19" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="Y19" t="str">
         <f t="shared" si="0"/>
@@ -3021,13 +3021,13 @@
         <v>28</v>
       </c>
       <c r="B21" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>357</v>
-      </c>
       <c r="D21" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>181</v>
@@ -3074,7 +3074,7 @@
         <v>45691</v>
       </c>
       <c r="U21" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="V21" s="4" t="s">
         <v>213</v>
@@ -3083,7 +3083,7 @@
         <v>186</v>
       </c>
       <c r="X21" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Y21" t="str">
         <f t="shared" si="0"/>
@@ -3124,7 +3124,7 @@
         <v>287</v>
       </c>
       <c r="V22" s="16" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="W22" s="16" t="s">
         <v>212</v>
@@ -3142,13 +3142,13 @@
         <v>29</v>
       </c>
       <c r="B23" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>357</v>
-      </c>
       <c r="D23" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>181</v>
@@ -3193,7 +3193,7 @@
         <v>45691</v>
       </c>
       <c r="U23" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="V23" s="4" t="s">
         <v>214</v>
@@ -3202,7 +3202,7 @@
         <v>186</v>
       </c>
       <c r="X23" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Y23" t="str">
         <f t="shared" si="0"/>
@@ -3256,13 +3256,13 @@
         <v>30</v>
       </c>
       <c r="B25" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>357</v>
-      </c>
       <c r="D25" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>181</v>
@@ -3318,7 +3318,7 @@
         <v>186</v>
       </c>
       <c r="X25" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Y25" t="str">
         <f t="shared" si="0"/>
@@ -3372,13 +3372,13 @@
         <v>31</v>
       </c>
       <c r="B27" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C27" s="15" t="s">
-        <v>357</v>
-      </c>
       <c r="D27" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>181</v>
@@ -3434,7 +3434,7 @@
         <v>186</v>
       </c>
       <c r="X27" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Y27" t="str">
         <f t="shared" si="0"/>
@@ -3476,7 +3476,7 @@
         <v>201</v>
       </c>
       <c r="V28" s="18" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="W28" s="16" t="s">
         <v>212</v>
@@ -3494,13 +3494,13 @@
         <v>33</v>
       </c>
       <c r="B29" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>357</v>
-      </c>
       <c r="D29" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>181</v>
@@ -3556,7 +3556,7 @@
         <v>186</v>
       </c>
       <c r="X29" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Y29" t="str">
         <f t="shared" si="0"/>
@@ -3620,13 +3620,13 @@
         <v>34</v>
       </c>
       <c r="B31" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C31" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C31" s="15" t="s">
-        <v>357</v>
-      </c>
       <c r="D31" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>181</v>
@@ -3682,7 +3682,7 @@
         <v>186</v>
       </c>
       <c r="X31" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Y31" t="str">
         <f t="shared" si="0"/>
@@ -3742,13 +3742,13 @@
         <v>37</v>
       </c>
       <c r="B33" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C33" s="15" t="s">
-        <v>357</v>
-      </c>
       <c r="D33" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>181</v>
@@ -3804,7 +3804,7 @@
         <v>186</v>
       </c>
       <c r="X33" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Y33" t="str">
         <f t="shared" si="0"/>
@@ -3864,13 +3864,13 @@
         <v>39</v>
       </c>
       <c r="B35" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C35" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C35" s="15" t="s">
-        <v>357</v>
-      </c>
       <c r="D35" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>181</v>
@@ -3926,7 +3926,7 @@
         <v>186</v>
       </c>
       <c r="X35" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Y35" t="str">
         <f t="shared" si="1"/>
@@ -3986,13 +3986,13 @@
         <v>40</v>
       </c>
       <c r="B37" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C37" s="15" t="s">
-        <v>357</v>
-      </c>
       <c r="D37" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>181</v>
@@ -4046,7 +4046,7 @@
         <v>186</v>
       </c>
       <c r="X37" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Y37" t="str">
         <f t="shared" si="1"/>
@@ -4085,10 +4085,10 @@
       <c r="S38" s="16"/>
       <c r="T38" s="19"/>
       <c r="U38" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="V38" s="16" t="s">
         <v>360</v>
-      </c>
-      <c r="V38" s="16" t="s">
-        <v>361</v>
       </c>
       <c r="W38" s="16" t="s">
         <v>212</v>
@@ -4106,13 +4106,13 @@
         <v>42</v>
       </c>
       <c r="B39" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C39" s="15" t="s">
-        <v>357</v>
-      </c>
       <c r="D39" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>181</v>
@@ -4168,7 +4168,7 @@
         <v>186</v>
       </c>
       <c r="X39" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Y39" t="str">
         <f t="shared" si="1"/>
@@ -4207,10 +4207,10 @@
       <c r="S40" s="16"/>
       <c r="T40" s="19"/>
       <c r="U40" s="16" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="V40" s="16" t="s">
-        <v>333</v>
+        <v>365</v>
       </c>
       <c r="W40" s="16" t="s">
         <v>212</v>
@@ -4228,13 +4228,13 @@
         <v>43</v>
       </c>
       <c r="B41" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="C41" s="17" t="s">
         <v>356</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>357</v>
-      </c>
       <c r="D41" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E41" s="16" t="s">
         <v>181</v>
@@ -4284,7 +4284,7 @@
         <v>186</v>
       </c>
       <c r="X41" s="16" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Y41" s="18" t="str">
         <f t="shared" si="1"/>
@@ -4338,13 +4338,13 @@
         <v>45</v>
       </c>
       <c r="B43" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C43" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C43" s="15" t="s">
-        <v>357</v>
-      </c>
       <c r="D43" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>181</v>
@@ -4402,7 +4402,7 @@
         <v>186</v>
       </c>
       <c r="X43" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Y43" t="str">
         <f t="shared" si="1"/>
@@ -4414,13 +4414,13 @@
         <v>24</v>
       </c>
       <c r="B44" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C44" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="D44" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>179</v>
@@ -4468,7 +4468,7 @@
         <v>189</v>
       </c>
       <c r="X44" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Y44" t="str">
         <f t="shared" si="1"/>
@@ -4480,13 +4480,13 @@
         <v>4</v>
       </c>
       <c r="B45" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C45" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="D45" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>179</v>
@@ -4542,7 +4542,7 @@
         <v>67</v>
       </c>
       <c r="X45" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y45" t="str">
         <f t="shared" si="1"/>
@@ -4554,13 +4554,13 @@
         <v>5</v>
       </c>
       <c r="B46" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C46" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="D46" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>179</v>
@@ -4616,7 +4616,7 @@
         <v>67</v>
       </c>
       <c r="X46" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y46" t="str">
         <f t="shared" si="1"/>
@@ -4628,13 +4628,13 @@
         <v>6</v>
       </c>
       <c r="B47" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C47" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="D47" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>179</v>
@@ -4690,7 +4690,7 @@
         <v>67</v>
       </c>
       <c r="X47" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y47" t="str">
         <f t="shared" si="1"/>
@@ -4702,13 +4702,13 @@
         <v>11</v>
       </c>
       <c r="B48" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C48" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="D48" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>179</v>
@@ -4764,7 +4764,7 @@
         <v>67</v>
       </c>
       <c r="X48" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y48" t="str">
         <f t="shared" si="1"/>
@@ -4776,13 +4776,13 @@
         <v>18</v>
       </c>
       <c r="B49" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C49" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="D49" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>179</v>
@@ -4838,7 +4838,7 @@
         <v>67</v>
       </c>
       <c r="X49" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y49" t="str">
         <f t="shared" si="1"/>
@@ -4850,13 +4850,13 @@
         <v>25</v>
       </c>
       <c r="B50" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C50" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="D50" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>179</v>
@@ -4914,7 +4914,7 @@
         <v>67</v>
       </c>
       <c r="X50" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y50" t="str">
         <f t="shared" si="1"/>
@@ -4926,13 +4926,13 @@
         <v>26</v>
       </c>
       <c r="B51" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C51" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="D51" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>179</v>
@@ -4984,7 +4984,7 @@
         <v>67</v>
       </c>
       <c r="X51" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y51" t="str">
         <f t="shared" si="1"/>
@@ -4996,10 +4996,10 @@
         <v>229</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>184</v>
@@ -5008,10 +5008,10 @@
         <v>249</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="R52" t="s">
         <v>50</v>
@@ -5026,7 +5026,7 @@
         <v>50</v>
       </c>
       <c r="X52" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y52" t="str">
         <f t="shared" si="1"/>
@@ -5038,10 +5038,10 @@
         <v>230</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>184</v>
@@ -5050,10 +5050,10 @@
         <v>249</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="R53" t="s">
         <v>50</v>
@@ -5068,7 +5068,7 @@
         <v>50</v>
       </c>
       <c r="X53" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y53" t="str">
         <f t="shared" si="1"/>
@@ -5080,10 +5080,10 @@
         <v>252</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>184</v>
@@ -5095,7 +5095,7 @@
         <v>251</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>251</v>
@@ -5131,7 +5131,7 @@
         <v>50</v>
       </c>
       <c r="X54" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y54" t="str">
         <f t="shared" si="1"/>
@@ -5143,10 +5143,10 @@
         <v>243</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F55" t="s">
         <v>184</v>
@@ -5158,7 +5158,7 @@
         <v>257</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J55" t="s">
         <v>257</v>
@@ -5194,7 +5194,7 @@
         <v>50</v>
       </c>
       <c r="X55" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y55" t="str">
         <f t="shared" si="1"/>
@@ -5206,10 +5206,10 @@
         <v>247</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F56" t="s">
         <v>184</v>
@@ -5221,7 +5221,7 @@
         <v>257</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J56" t="s">
         <v>257</v>
@@ -5242,7 +5242,7 @@
         <v>50</v>
       </c>
       <c r="X56" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y56" t="str">
         <f t="shared" si="1"/>
@@ -5254,10 +5254,10 @@
         <v>231</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F57" t="s">
         <v>184</v>
@@ -5269,7 +5269,7 @@
         <v>257</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J57" t="s">
         <v>257</v>
@@ -5305,7 +5305,7 @@
         <v>50</v>
       </c>
       <c r="X57" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y57" t="str">
         <f t="shared" si="1"/>
@@ -5317,10 +5317,10 @@
         <v>248</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F58" t="s">
         <v>184</v>
@@ -5332,7 +5332,7 @@
         <v>257</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J58" t="s">
         <v>257</v>
@@ -5353,7 +5353,7 @@
         <v>50</v>
       </c>
       <c r="X58" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y58" t="str">
         <f t="shared" si="1"/>
@@ -5365,10 +5365,10 @@
         <v>238</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F59" t="s">
         <v>184</v>
@@ -5380,7 +5380,7 @@
         <v>257</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J59" t="s">
         <v>257</v>
@@ -5416,7 +5416,7 @@
         <v>50</v>
       </c>
       <c r="X59" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y59" t="str">
         <f t="shared" si="1"/>
@@ -5428,10 +5428,10 @@
         <v>239</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F60" t="s">
         <v>184</v>
@@ -5443,7 +5443,7 @@
         <v>257</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J60" t="s">
         <v>257</v>
@@ -5479,7 +5479,7 @@
         <v>50</v>
       </c>
       <c r="X60" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y60" t="str">
         <f t="shared" si="1"/>
@@ -5491,10 +5491,10 @@
         <v>236</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F61" t="s">
         <v>184</v>
@@ -5506,7 +5506,7 @@
         <v>257</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J61" t="s">
         <v>257</v>
@@ -5542,7 +5542,7 @@
         <v>50</v>
       </c>
       <c r="X61" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y61" t="str">
         <f t="shared" si="1"/>
@@ -5554,10 +5554,10 @@
         <v>232</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D62" s="8"/>
       <c r="F62" t="s">
@@ -5570,7 +5570,7 @@
         <v>257</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J62" t="s">
         <v>257</v>
@@ -5606,7 +5606,7 @@
         <v>50</v>
       </c>
       <c r="X62" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y62" t="str">
         <f t="shared" si="1"/>
@@ -5618,10 +5618,10 @@
         <v>245</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D63" s="8"/>
       <c r="F63" t="s">
@@ -5634,7 +5634,7 @@
         <v>257</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J63" t="s">
         <v>257</v>
@@ -5670,7 +5670,7 @@
         <v>50</v>
       </c>
       <c r="X63" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y63" t="str">
         <f t="shared" si="1"/>
@@ -5682,10 +5682,10 @@
         <v>240</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F64" t="s">
         <v>184</v>
@@ -5697,7 +5697,7 @@
         <v>257</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J64" t="s">
         <v>257</v>
@@ -5733,7 +5733,7 @@
         <v>50</v>
       </c>
       <c r="X64" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y64" t="str">
         <f t="shared" si="1"/>
@@ -5745,10 +5745,10 @@
         <v>241</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F65" t="s">
         <v>184</v>
@@ -5760,7 +5760,7 @@
         <v>257</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J65" t="s">
         <v>257</v>
@@ -5796,7 +5796,7 @@
         <v>50</v>
       </c>
       <c r="X65" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y65" t="str">
         <f t="shared" si="1"/>
@@ -5808,10 +5808,10 @@
         <v>235</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F66" t="s">
         <v>184</v>
@@ -5823,7 +5823,7 @@
         <v>257</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J66" t="s">
         <v>257</v>
@@ -5862,7 +5862,7 @@
         <v>50</v>
       </c>
       <c r="X66" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y66" t="str">
         <f t="shared" ref="Y66:Y72" si="2">CONCATENATE(U66, " (", W66, ")")</f>
@@ -5874,10 +5874,10 @@
         <v>244</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D67" s="9"/>
       <c r="F67" t="s">
@@ -5890,7 +5890,7 @@
         <v>257</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J67" t="s">
         <v>257</v>
@@ -5911,7 +5911,7 @@
         <v>50</v>
       </c>
       <c r="X67" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y67" t="str">
         <f t="shared" si="2"/>
@@ -5923,10 +5923,10 @@
         <v>233</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D68" s="9"/>
       <c r="F68" t="s">
@@ -5939,7 +5939,7 @@
         <v>257</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J68" t="s">
         <v>257</v>
@@ -5975,7 +5975,7 @@
         <v>50</v>
       </c>
       <c r="X68" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y68" t="str">
         <f t="shared" si="2"/>
@@ -5987,10 +5987,10 @@
         <v>246</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F69" t="s">
         <v>184</v>
@@ -6002,7 +6002,7 @@
         <v>257</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J69" t="s">
         <v>257</v>
@@ -6038,7 +6038,7 @@
         <v>50</v>
       </c>
       <c r="X69" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y69" t="str">
         <f t="shared" si="2"/>
@@ -6050,10 +6050,10 @@
         <v>242</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F70" t="s">
         <v>184</v>
@@ -6065,7 +6065,7 @@
         <v>257</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J70" t="s">
         <v>257</v>
@@ -6101,7 +6101,7 @@
         <v>50</v>
       </c>
       <c r="X70" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y70" t="str">
         <f t="shared" si="2"/>
@@ -6113,10 +6113,10 @@
         <v>237</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F71" t="s">
         <v>184</v>
@@ -6128,7 +6128,7 @@
         <v>257</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J71" t="s">
         <v>257</v>
@@ -6164,7 +6164,7 @@
         <v>50</v>
       </c>
       <c r="X71" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y71" t="str">
         <f t="shared" si="2"/>
@@ -6176,10 +6176,10 @@
         <v>234</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F72" t="s">
         <v>184</v>
@@ -6191,7 +6191,7 @@
         <v>276</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J72" t="s">
         <v>276</v>
@@ -6227,7 +6227,7 @@
         <v>50</v>
       </c>
       <c r="X72" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y72" t="str">
         <f t="shared" si="2"/>

</xml_diff>